<commit_message>
comment function, other bug fix
</commit_message>
<xml_diff>
--- a/polls/IROS20_Sessions_Chairs.xlsx
+++ b/polls/IROS20_Sessions_Chairs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akdba\Desktop\mysite\polls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AE3C52-2961-4809-A3A1-A2C9F7904E57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA9F395-8527-4377-97C0-0BCC13AAB841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4238" uniqueCount="1992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4239" uniqueCount="1992">
   <si>
     <t>Role</t>
   </si>
@@ -6409,8 +6409,8 @@
   </sheetPr>
   <dimension ref="A1:V975"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="C211" sqref="C211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14645,7 +14645,9 @@
       <c r="A211" s="21" t="s">
         <v>317</v>
       </c>
-      <c r="B211" s="9"/>
+      <c r="B211" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="C211" s="9"/>
       <c r="D211" s="9"/>
       <c r="E211" s="3"/>

</xml_diff>